<commit_message>
remake the charts, xls/odg fu
git-svn-id: https://tor.ern.nps.edu/svn/proj/labtainer/trunk@2073 ed162e55-3153-4343-a18d-e086fa355ed4
</commit_message>
<xml_diff>
--- a/labs/backups2/docs/backups-Input.xlsx
+++ b/labs/backups2/docs/backups-Input.xlsx
@@ -263,16 +263,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0%"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -312,23 +310,13 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="13"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -342,7 +330,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD7E4BD"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -384,7 +372,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -445,14 +433,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -478,8 +458,8 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF878787"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -487,7 +467,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFA4C1FF"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -504,7 +484,7 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3E7FCC"/>
+      <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
@@ -512,7 +492,7 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -525,7 +505,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -537,7 +517,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="1" sz="1800" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -546,11 +526,11 @@
                     <a:srgbClr val="ffffff"/>
                   </a:solidFill>
                 </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="1" sz="1800" spc="-1" strike="noStrike">
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -559,7 +539,7 @@
                     <a:srgbClr val="ffffff"/>
                   </a:solidFill>
                 </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Backup Rates</a:t>
             </a:r>
@@ -578,13 +558,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -652,13 +634,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="69349195"/>
-        <c:axId val="4800305"/>
+        <c:axId val="78347236"/>
+        <c:axId val="25331557"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="69349195"/>
+        <c:axId val="78347236"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,11 +651,10 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="9360">
+          <a:ln>
             <a:solidFill>
-              <a:srgbClr val="878787"/>
+              <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
-            <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -689,19 +670,19 @@
                     <a:srgbClr val="ffffff"/>
                   </a:solidFill>
                 </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4800305"/>
+        <c:crossAx val="25331557"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4800305"/>
+        <c:axId val="25331557"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -709,62 +690,22 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9360">
+            <a:ln>
               <a:solidFill>
-                <a:srgbClr val="878787"/>
+                <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Bytes / Second</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)" sourceLinked="0"/>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="9360">
+          <a:ln>
             <a:solidFill>
-              <a:srgbClr val="878787"/>
+              <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
-            <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -780,21 +721,21 @@
                     <a:srgbClr val="ffffff"/>
                   </a:solidFill>
                 </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69349195"/>
+        <c:crossAx val="78347236"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
+        <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
         </a:ln>
       </c:spPr>
     </c:plotArea>
@@ -812,7 +753,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -824,7 +765,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="1" sz="1800" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -833,11 +774,11 @@
                     <a:srgbClr val="ffffff"/>
                   </a:solidFill>
                 </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="1" sz="1800" spc="-1" strike="noStrike">
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -846,7 +787,7 @@
                     <a:srgbClr val="ffffff"/>
                   </a:solidFill>
                 </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Time per TB</a:t>
             </a:r>
@@ -865,13 +806,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -939,13 +882,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="24193489"/>
-        <c:axId val="40146887"/>
+        <c:axId val="14301596"/>
+        <c:axId val="66761153"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="24193489"/>
+        <c:axId val="14301596"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,11 +899,10 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="9360">
+          <a:ln>
             <a:solidFill>
-              <a:srgbClr val="878787"/>
+              <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
-            <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -976,19 +918,19 @@
                     <a:srgbClr val="ffffff"/>
                   </a:solidFill>
                 </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40146887"/>
+        <c:crossAx val="66761153"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40146887"/>
+        <c:axId val="66761153"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -996,62 +938,22 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9360">
+            <a:ln>
               <a:solidFill>
-                <a:srgbClr val="878787"/>
+                <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Hours</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)" sourceLinked="0"/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="9360">
+          <a:ln>
             <a:solidFill>
-              <a:srgbClr val="878787"/>
+              <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
-            <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -1067,21 +969,21 @@
                     <a:srgbClr val="ffffff"/>
                   </a:solidFill>
                 </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24193489"/>
+        <c:crossAx val="14301596"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
+        <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
         </a:ln>
       </c:spPr>
     </c:plotArea>
@@ -1103,25 +1005,25 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>59040</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>193680</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>428400</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>408960</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvPr id="0" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8555040" y="3139920"/>
-        <a:ext cx="5751000" cy="4254120"/>
+        <a:off x="8051760" y="2192760"/>
+        <a:ext cx="5768280" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1133,25 +1035,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>820080</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>513000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>734400</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>719640</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 2"/>
+        <xdr:cNvPr id="1" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9316080" y="8279640"/>
-        <a:ext cx="5295960" cy="2921040"/>
+        <a:off x="8371080" y="8082720"/>
+        <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1171,21 +1073,21 @@
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.1813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.506976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.2418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.1627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1662,7 +1564,7 @@
       <c r="C34" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="15" t="n">
+      <c r="D34" s="13" t="n">
         <f aca="false">IF(D13&lt;&gt;0,(D13-D31)/D13,0)</f>
         <v>0</v>
       </c>
@@ -1675,7 +1577,7 @@
       <c r="C35" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="15" t="n">
+      <c r="D35" s="13" t="n">
         <f aca="false">IF(D11&lt;&gt;0,(D30-D11)/D11,0)</f>
         <v>0</v>
       </c>
@@ -1777,7 +1679,7 @@
       <c r="C42" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="16" t="n">
+      <c r="D42" s="14" t="n">
         <f aca="false">IF(D4&lt;&gt;0,(D39*I39)/(D4*3600),0)</f>
         <v>6108397.93208889</v>
       </c>

</xml_diff>